<commit_message>
Ajustes Archivos Fase 2
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de documentación/Informe de Pruebas de Funcionalidad.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de documentación/Informe de Pruebas de Funcionalidad.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -134,7 +134,10 @@
     <t xml:space="preserve">Se enviara un correo a las cuentas de asuntos estudiantiles informando si se elimino o creo una votacion con la respectiva sigla de esta  </t>
   </si>
   <si>
-    <t>Funciona sin ningun problema - Sin Observaciones - Se encuentra y sugiere que no solo le llegue correo a los de asuntos estudiantiles si no que tambien a los concejeros de carrera</t>
+    <t>Funciona sin ningun problema - Sin Observaciones - Se encuentra y sugiere que no solo le llegue correo a los de asuntos estudiantiles si no que tambien a los consejeros de carrera</t>
+  </si>
+  <si>
+    <t>Se añade a la funcion de notificacion de correos que cuando se cree o elimine se avise tanto a usuarios de asuntos estudiantiles y a consejeros de carrera</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1627,9 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="4"/>
-      <c r="V23" s="12"/>
+      <c r="V23" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="W23" s="3"/>
       <c r="X23" s="4"/>
     </row>

</xml_diff>